<commit_message>
Genes Supplement - Removed CD152 (== CTLA4) and added Set5 (all proteins (19962))
</commit_message>
<xml_diff>
--- a/Supplement/genesReferencesFeatureSetsNumbered.xlsx
+++ b/Supplement/genesReferencesFeatureSetsNumbered.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/801a5cf5c13d3b0a/Documents/-= Hogeschool Rotterdam =-/39_ExploratorySoftwareDevelopment/Capstone/20250518_tenthAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\000_Projecten\HogeschoolRotterdam\ExploratoryDevelopmentCapstone\Supplement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1800" documentId="11_F25DC773A252ABDACC10485EB159563E5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D654C419-0D1F-49D4-902F-A5AA4676F433}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D19A4C2-9641-4ADF-B83E-89B30B4B2748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="FeatureSet2" sheetId="4" r:id="rId5"/>
     <sheet name="FeatureSet3" sheetId="5" r:id="rId6"/>
     <sheet name="FeatureSet4" sheetId="6" r:id="rId7"/>
+    <sheet name="FeatureSet5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="413">
   <si>
     <t>s10911-023-09540-2</t>
   </si>
@@ -1275,6 +1276,12 @@
   </si>
   <si>
     <t>All genes mentioned on sheet "GeneAndReference"</t>
+  </si>
+  <si>
+    <t>All proteins</t>
+  </si>
+  <si>
+    <t>Count ==</t>
   </si>
 </sst>
 </file>
@@ -1422,8 +1429,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1707,7 +1714,7 @@
   <dimension ref="B2:T295"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E176" sqref="E176"/>
+      <selection activeCell="F170" sqref="F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,7 +2390,7 @@
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B48" s="9">
-        <f t="shared" ref="B48:B62" si="1">COUNTA(D48:AA48)</f>
+        <f t="shared" ref="B48:B61" si="1">COUNTA(D48:AA48)</f>
         <v>1</v>
       </c>
       <c r="C48" t="s">
@@ -4303,7 +4310,7 @@
     </row>
     <row r="180" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B180" s="9">
-        <f t="shared" ref="B180:B194" si="8">COUNTA(D180:AA180)</f>
+        <f t="shared" ref="B180:B193" si="8">COUNTA(D180:AA180)</f>
         <v>2</v>
       </c>
       <c r="C180" t="s">
@@ -6051,7 +6058,7 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
-        <f>COUNTA(D7:AA7)</f>
+        <f t="shared" ref="B7:B70" si="0">COUNTA(D7:AA7)</f>
         <v>17</v>
       </c>
       <c r="C7" t="s">
@@ -6111,7 +6118,7 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
-        <f>COUNTA(D8:AA8)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C8" t="s">
@@ -6162,7 +6169,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
-        <f>COUNTA(D9:AA9)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C9" t="s">
@@ -6213,7 +6220,7 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
-        <f>COUNTA(D10:AA10)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C10" t="s">
@@ -6264,7 +6271,7 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
-        <f>COUNTA(D11:AA11)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C11" t="s">
@@ -6315,7 +6322,7 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
-        <f>COUNTA(D12:AA12)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C12" t="s">
@@ -6354,7 +6361,7 @@
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
-        <f>COUNTA(D13:AA13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C13" t="s">
@@ -6393,7 +6400,7 @@
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
-        <f>COUNTA(D14:AA14)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C14" t="s">
@@ -6426,7 +6433,7 @@
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
-        <f>COUNTA(D15:AA15)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C15" t="s">
@@ -6459,7 +6466,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
-        <f>COUNTA(D16:AA16)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" t="s">
@@ -6489,7 +6496,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
-        <f>COUNTA(D17:AA17)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C17" t="s">
@@ -6519,7 +6526,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
-        <f>COUNTA(D18:AA18)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C18" t="s">
@@ -6549,7 +6556,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
-        <f>COUNTA(D19:AA19)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C19" t="s">
@@ -6579,7 +6586,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
-        <f>COUNTA(D20:AA20)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C20" t="s">
@@ -6606,7 +6613,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
-        <f>COUNTA(D21:AA21)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C21" t="s">
@@ -6633,7 +6640,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
-        <f>COUNTA(D22:AA22)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -6660,7 +6667,7 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="9">
-        <f>COUNTA(D23:AA23)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C23" t="s">
@@ -6687,7 +6694,7 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="9">
-        <f>COUNTA(D24:AA24)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C24" t="s">
@@ -6714,7 +6721,7 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
-        <f>COUNTA(D25:AA25)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C25" t="s">
@@ -6738,7 +6745,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="9">
-        <f>COUNTA(D26:AA26)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C26" t="s">
@@ -6762,7 +6769,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="9">
-        <f>COUNTA(D27:AA27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -6786,7 +6793,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="9">
-        <f>COUNTA(D28:AA28)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C28" t="s">
@@ -6810,7 +6817,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="9">
-        <f>COUNTA(D29:AA29)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C29" t="s">
@@ -6831,7 +6838,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="9">
-        <f>COUNTA(D30:AA30)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C30" t="s">
@@ -6852,7 +6859,7 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="9">
-        <f>COUNTA(D31:AA31)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C31" t="s">
@@ -6873,7 +6880,7 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="9">
-        <f>COUNTA(D32:AA32)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C32" t="s">
@@ -6894,7 +6901,7 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="9">
-        <f>COUNTA(D33:AA33)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C33" t="s">
@@ -6915,7 +6922,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="9">
-        <f>COUNTA(D34:AA34)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C34" t="s">
@@ -6936,7 +6943,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="9">
-        <f>COUNTA(D35:AA35)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C35" t="s">
@@ -6957,7 +6964,7 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="9">
-        <f>COUNTA(D36:AA36)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C36" t="s">
@@ -6978,7 +6985,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="9">
-        <f>COUNTA(D37:AA37)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C37" t="s">
@@ -6999,7 +7006,7 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="9">
-        <f>COUNTA(D38:AA38)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -7020,7 +7027,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="9">
-        <f>COUNTA(D39:AA39)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C39" t="s">
@@ -7038,7 +7045,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="9">
-        <f>COUNTA(D40:AA40)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C40" t="s">
@@ -7056,7 +7063,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="9">
-        <f>COUNTA(D41:AA41)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C41" t="s">
@@ -7074,7 +7081,7 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="9">
-        <f>COUNTA(D42:AA42)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C42" t="s">
@@ -7092,7 +7099,7 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="9">
-        <f>COUNTA(D43:AA43)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C43" t="s">
@@ -7110,7 +7117,7 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="9">
-        <f>COUNTA(D44:AA44)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C44" t="s">
@@ -7128,7 +7135,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="9">
-        <f>COUNTA(D45:AA45)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C45" t="s">
@@ -7146,7 +7153,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="9">
-        <f>COUNTA(D46:AA46)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C46" t="s">
@@ -7164,7 +7171,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="9">
-        <f>COUNTA(D47:AA47)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -7182,7 +7189,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="9">
-        <f>COUNTA(D48:AA48)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C48" t="s">
@@ -7200,7 +7207,7 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="9">
-        <f>COUNTA(D49:AA49)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C49" t="s">
@@ -7218,7 +7225,7 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="9">
-        <f>COUNTA(D50:AA50)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C50" t="s">
@@ -7236,7 +7243,7 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="9">
-        <f>COUNTA(D51:AA51)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C51" t="s">
@@ -7254,7 +7261,7 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="9">
-        <f>COUNTA(D52:AA52)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C52" t="s">
@@ -7272,7 +7279,7 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="9">
-        <f>COUNTA(D53:AA53)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C53" t="s">
@@ -7287,7 +7294,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="9">
-        <f>COUNTA(D54:AA54)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C54" t="s">
@@ -7302,7 +7309,7 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="9">
-        <f>COUNTA(D55:AA55)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C55" t="s">
@@ -7317,7 +7324,7 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="9">
-        <f>COUNTA(D56:AA56)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C56" t="s">
@@ -7332,7 +7339,7 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="9">
-        <f>COUNTA(D57:AA57)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C57" t="s">
@@ -7347,7 +7354,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="9">
-        <f>COUNTA(D58:AA58)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C58" t="s">
@@ -7362,7 +7369,7 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="9">
-        <f>COUNTA(D59:AA59)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C59" t="s">
@@ -7377,7 +7384,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="9">
-        <f>COUNTA(D60:AA60)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C60" t="s">
@@ -7392,7 +7399,7 @@
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="9">
-        <f>COUNTA(D61:AA61)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C61" t="s">
@@ -7407,7 +7414,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="9">
-        <f>COUNTA(D62:AA62)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C62" t="s">
@@ -7422,7 +7429,7 @@
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="9">
-        <f>COUNTA(D63:AA63)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C63" t="s">
@@ -7437,7 +7444,7 @@
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="9">
-        <f>COUNTA(D64:AA64)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -7452,7 +7459,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="9">
-        <f>COUNTA(D65:AA65)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C65" t="s">
@@ -7467,7 +7474,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="9">
-        <f>COUNTA(D66:AA66)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C66" t="s">
@@ -7482,7 +7489,7 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="9">
-        <f>COUNTA(D67:AA67)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C67" t="s">
@@ -7497,7 +7504,7 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="9">
-        <f>COUNTA(D68:AA68)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C68" t="s">
@@ -7512,7 +7519,7 @@
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="9">
-        <f>COUNTA(D69:AA69)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C69" t="s">
@@ -7527,7 +7534,7 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="9">
-        <f>COUNTA(D70:AA70)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C70" t="s">
@@ -7542,7 +7549,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="9">
-        <f>COUNTA(D71:AA71)</f>
+        <f t="shared" ref="B71:B134" si="1">COUNTA(D71:AA71)</f>
         <v>2</v>
       </c>
       <c r="C71" t="s">
@@ -7557,7 +7564,7 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="9">
-        <f>COUNTA(D72:AA72)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C72" t="s">
@@ -7572,7 +7579,7 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="9">
-        <f>COUNTA(D73:AA73)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C73" t="s">
@@ -7587,7 +7594,7 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="9">
-        <f>COUNTA(D74:AA74)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C74" t="s">
@@ -7602,7 +7609,7 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="9">
-        <f>COUNTA(D75:AA75)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C75" t="s">
@@ -7617,7 +7624,7 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="9">
-        <f>COUNTA(D76:AA76)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C76" t="s">
@@ -7632,7 +7639,7 @@
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="9">
-        <f>COUNTA(D77:AA77)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C77" t="s">
@@ -7647,7 +7654,7 @@
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="9">
-        <f>COUNTA(D78:AA78)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C78" t="s">
@@ -7662,7 +7669,7 @@
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="9">
-        <f>COUNTA(D79:AA79)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C79" t="s">
@@ -7677,7 +7684,7 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="9">
-        <f>COUNTA(D80:AA80)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C80" t="s">
@@ -7692,7 +7699,7 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="9">
-        <f>COUNTA(D81:AA81)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C81" t="s">
@@ -7707,7 +7714,7 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="9">
-        <f>COUNTA(D82:AA82)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C82" t="s">
@@ -7722,7 +7729,7 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="9">
-        <f>COUNTA(D83:AA83)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C83" t="s">
@@ -7737,7 +7744,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="9">
-        <f>COUNTA(D84:AA84)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C84" t="s">
@@ -7752,7 +7759,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="9">
-        <f>COUNTA(D85:AA85)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C85" t="s">
@@ -7767,7 +7774,7 @@
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="9">
-        <f>COUNTA(D86:AA86)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C86" t="s">
@@ -7782,7 +7789,7 @@
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="9">
-        <f>COUNTA(D87:AA87)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C87" t="s">
@@ -7794,7 +7801,7 @@
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="9">
-        <f>COUNTA(D88:AA88)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C88" t="s">
@@ -7806,7 +7813,7 @@
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="9">
-        <f>COUNTA(D89:AA89)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C89" t="s">
@@ -7818,7 +7825,7 @@
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="9">
-        <f>COUNTA(D90:AA90)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C90" t="s">
@@ -7830,7 +7837,7 @@
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="9">
-        <f>COUNTA(D91:AA91)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C91" t="s">
@@ -7842,7 +7849,7 @@
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="9">
-        <f>COUNTA(D92:AA92)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C92" t="s">
@@ -7854,7 +7861,7 @@
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="9">
-        <f>COUNTA(D93:AA93)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C93" t="s">
@@ -7866,7 +7873,7 @@
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="9">
-        <f>COUNTA(D94:AA94)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C94" t="s">
@@ -7878,7 +7885,7 @@
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="9">
-        <f>COUNTA(D95:AA95)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C95" t="s">
@@ -7890,7 +7897,7 @@
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="9">
-        <f>COUNTA(D96:AA96)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C96" t="s">
@@ -7902,7 +7909,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="9">
-        <f>COUNTA(D97:AA97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C97" t="s">
@@ -7914,7 +7921,7 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="9">
-        <f>COUNTA(D98:AA98)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C98" t="s">
@@ -7926,7 +7933,7 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="9">
-        <f>COUNTA(D99:AA99)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C99" t="s">
@@ -7938,7 +7945,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="9">
-        <f>COUNTA(D100:AA100)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C100" t="s">
@@ -7950,7 +7957,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="9">
-        <f>COUNTA(D101:AA101)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C101" t="s">
@@ -7962,7 +7969,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="9">
-        <f>COUNTA(D102:AA102)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C102" t="s">
@@ -7974,7 +7981,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="9">
-        <f>COUNTA(D103:AA103)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C103" t="s">
@@ -7986,7 +7993,7 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="9">
-        <f>COUNTA(D104:AA104)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C104" t="s">
@@ -7998,7 +8005,7 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="9">
-        <f>COUNTA(D105:AA105)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C105" t="s">
@@ -8010,7 +8017,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" s="9">
-        <f>COUNTA(D106:AA106)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C106" t="s">
@@ -8022,7 +8029,7 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" s="9">
-        <f>COUNTA(D107:AA107)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C107" t="s">
@@ -8034,7 +8041,7 @@
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" s="9">
-        <f>COUNTA(D108:AA108)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C108" t="s">
@@ -8046,7 +8053,7 @@
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109" s="9">
-        <f>COUNTA(D109:AA109)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C109" t="s">
@@ -8058,7 +8065,7 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" s="9">
-        <f>COUNTA(D110:AA110)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C110" t="s">
@@ -8070,7 +8077,7 @@
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" s="9">
-        <f>COUNTA(D111:AA111)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C111" t="s">
@@ -8082,7 +8089,7 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" s="9">
-        <f>COUNTA(D112:AA112)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C112" t="s">
@@ -8094,7 +8101,7 @@
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" s="9">
-        <f>COUNTA(D113:AA113)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C113" t="s">
@@ -8106,7 +8113,7 @@
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" s="9">
-        <f>COUNTA(D114:AA114)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C114" t="s">
@@ -8118,7 +8125,7 @@
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" s="9">
-        <f>COUNTA(D115:AA115)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C115" t="s">
@@ -8130,7 +8137,7 @@
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" s="9">
-        <f>COUNTA(D116:AA116)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C116" t="s">
@@ -8142,7 +8149,7 @@
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" s="9">
-        <f>COUNTA(D117:AA117)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C117" t="s">
@@ -8154,7 +8161,7 @@
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" s="9">
-        <f>COUNTA(D118:AA118)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C118" t="s">
@@ -8166,7 +8173,7 @@
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" s="9">
-        <f>COUNTA(D119:AA119)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C119" t="s">
@@ -8178,7 +8185,7 @@
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" s="9">
-        <f>COUNTA(D120:AA120)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C120" t="s">
@@ -8190,7 +8197,7 @@
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" s="9">
-        <f>COUNTA(D121:AA121)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C121" t="s">
@@ -8202,7 +8209,7 @@
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" s="9">
-        <f>COUNTA(D122:AA122)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C122" t="s">
@@ -8214,7 +8221,7 @@
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" s="9">
-        <f>COUNTA(D123:AA123)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C123" t="s">
@@ -8226,7 +8233,7 @@
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" s="9">
-        <f>COUNTA(D124:AA124)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C124" t="s">
@@ -8238,7 +8245,7 @@
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B125" s="9">
-        <f>COUNTA(D125:AA125)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C125" t="s">
@@ -8250,7 +8257,7 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B126" s="9">
-        <f>COUNTA(D126:AA126)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C126" t="s">
@@ -8262,7 +8269,7 @@
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B127" s="9">
-        <f>COUNTA(D127:AA127)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C127" t="s">
@@ -8274,7 +8281,7 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" s="9">
-        <f>COUNTA(D128:AA128)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C128" t="s">
@@ -8286,7 +8293,7 @@
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="9">
-        <f>COUNTA(D129:AA129)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C129" t="s">
@@ -8298,7 +8305,7 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130" s="9">
-        <f>COUNTA(D130:AA130)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C130" t="s">
@@ -8310,7 +8317,7 @@
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="9">
-        <f>COUNTA(D131:AA131)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C131" t="s">
@@ -8322,7 +8329,7 @@
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="9">
-        <f>COUNTA(D132:AA132)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C132" t="s">
@@ -8334,7 +8341,7 @@
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133" s="9">
-        <f>COUNTA(D133:AA133)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C133" t="s">
@@ -8346,7 +8353,7 @@
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134" s="9">
-        <f>COUNTA(D134:AA134)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C134" t="s">
@@ -8358,7 +8365,7 @@
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="9">
-        <f>COUNTA(D135:AA135)</f>
+        <f t="shared" ref="B135:B198" si="2">COUNTA(D135:AA135)</f>
         <v>1</v>
       </c>
       <c r="C135" t="s">
@@ -8370,7 +8377,7 @@
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B136" s="9">
-        <f>COUNTA(D136:AA136)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C136" t="s">
@@ -8382,7 +8389,7 @@
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B137" s="9">
-        <f>COUNTA(D137:AA137)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C137" t="s">
@@ -8394,7 +8401,7 @@
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B138" s="9">
-        <f>COUNTA(D138:AA138)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C138" t="s">
@@ -8406,7 +8413,7 @@
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B139" s="9">
-        <f>COUNTA(D139:AA139)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C139" t="s">
@@ -8418,7 +8425,7 @@
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B140" s="9">
-        <f>COUNTA(D140:AA140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C140" t="s">
@@ -8430,7 +8437,7 @@
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B141" s="9">
-        <f>COUNTA(D141:AA141)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C141" t="s">
@@ -8442,7 +8449,7 @@
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B142" s="9">
-        <f>COUNTA(D142:AA142)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C142" t="s">
@@ -8454,7 +8461,7 @@
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="9">
-        <f>COUNTA(D143:AA143)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C143" t="s">
@@ -8466,7 +8473,7 @@
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="9">
-        <f>COUNTA(D144:AA144)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C144" t="s">
@@ -8478,7 +8485,7 @@
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B145" s="9">
-        <f>COUNTA(D145:AA145)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C145" t="s">
@@ -8490,7 +8497,7 @@
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="9">
-        <f>COUNTA(D146:AA146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C146" t="s">
@@ -8502,7 +8509,7 @@
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B147" s="9">
-        <f>COUNTA(D147:AA147)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C147" t="s">
@@ -8514,7 +8521,7 @@
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B148" s="9">
-        <f>COUNTA(D148:AA148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C148" t="s">
@@ -8526,7 +8533,7 @@
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B149" s="9">
-        <f>COUNTA(D149:AA149)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C149" t="s">
@@ -8538,7 +8545,7 @@
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B150" s="9">
-        <f>COUNTA(D150:AA150)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C150" t="s">
@@ -8550,7 +8557,7 @@
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B151" s="9">
-        <f>COUNTA(D151:AA151)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C151" t="s">
@@ -8562,7 +8569,7 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B152" s="9">
-        <f>COUNTA(D152:AA152)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C152" t="s">
@@ -8574,7 +8581,7 @@
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B153" s="9">
-        <f>COUNTA(D153:AA153)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C153" t="s">
@@ -8586,7 +8593,7 @@
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B154" s="9">
-        <f>COUNTA(D154:AA154)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
@@ -8598,7 +8605,7 @@
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B155" s="9">
-        <f>COUNTA(D155:AA155)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C155" t="s">
@@ -8610,7 +8617,7 @@
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B156" s="9">
-        <f>COUNTA(D156:AA156)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C156" t="s">
@@ -8622,7 +8629,7 @@
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B157" s="9">
-        <f>COUNTA(D157:AA157)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C157" t="s">
@@ -8634,7 +8641,7 @@
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B158" s="9">
-        <f>COUNTA(D158:AA158)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C158" t="s">
@@ -8646,7 +8653,7 @@
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B159" s="9">
-        <f>COUNTA(D159:AA159)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C159" t="s">
@@ -8658,7 +8665,7 @@
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B160" s="9">
-        <f>COUNTA(D160:AA160)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C160" t="s">
@@ -8670,7 +8677,7 @@
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B161" s="9">
-        <f>COUNTA(D161:AA161)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C161" t="s">
@@ -8682,7 +8689,7 @@
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B162" s="9">
-        <f>COUNTA(D162:AA162)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C162" t="s">
@@ -8694,7 +8701,7 @@
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B163" s="9">
-        <f>COUNTA(D163:AA163)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C163" t="s">
@@ -8706,7 +8713,7 @@
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B164" s="9">
-        <f>COUNTA(D164:AA164)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C164" t="s">
@@ -8718,7 +8725,7 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B165" s="9">
-        <f>COUNTA(D165:AA165)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C165" t="s">
@@ -8730,7 +8737,7 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B166" s="9">
-        <f>COUNTA(D166:AA166)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C166" t="s">
@@ -8742,7 +8749,7 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B167" s="9">
-        <f>COUNTA(D167:AA167)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C167" t="s">
@@ -8754,7 +8761,7 @@
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B168" s="9">
-        <f>COUNTA(D168:AA168)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C168" t="s">
@@ -8766,7 +8773,7 @@
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B169" s="9">
-        <f>COUNTA(D169:AA169)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C169" t="s">
@@ -8778,7 +8785,7 @@
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B170" s="9">
-        <f>COUNTA(D170:AA170)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C170" t="s">
@@ -8790,7 +8797,7 @@
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B171" s="9">
-        <f>COUNTA(D171:AA171)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C171" t="s">
@@ -8802,7 +8809,7 @@
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B172" s="9">
-        <f>COUNTA(D172:AA172)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C172" t="s">
@@ -8814,7 +8821,7 @@
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B173" s="9">
-        <f>COUNTA(D173:AA173)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C173" t="s">
@@ -8826,7 +8833,7 @@
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B174" s="9">
-        <f>COUNTA(D174:AA174)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C174" t="s">
@@ -8838,7 +8845,7 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B175" s="9">
-        <f>COUNTA(D175:AA175)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C175" t="s">
@@ -8850,7 +8857,7 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B176" s="9">
-        <f>COUNTA(D176:AA176)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C176" t="s">
@@ -8862,7 +8869,7 @@
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B177" s="9">
-        <f>COUNTA(D177:AA177)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C177" t="s">
@@ -8874,7 +8881,7 @@
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B178" s="9">
-        <f>COUNTA(D178:AA178)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C178" t="s">
@@ -8886,7 +8893,7 @@
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B179" s="9">
-        <f>COUNTA(D179:AA179)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C179" t="s">
@@ -8898,7 +8905,7 @@
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B180" s="9">
-        <f>COUNTA(D180:AA180)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C180" t="s">
@@ -8910,7 +8917,7 @@
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B181" s="9">
-        <f>COUNTA(D181:AA181)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C181" t="s">
@@ -8922,7 +8929,7 @@
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B182" s="9">
-        <f>COUNTA(D182:AA182)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C182" t="s">
@@ -8934,7 +8941,7 @@
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B183" s="9">
-        <f>COUNTA(D183:AA183)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C183" t="s">
@@ -8946,7 +8953,7 @@
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B184" s="9">
-        <f>COUNTA(D184:AA184)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C184" s="3" t="s">
@@ -8958,7 +8965,7 @@
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B185" s="9">
-        <f>COUNTA(D185:AA185)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C185" t="s">
@@ -8970,7 +8977,7 @@
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B186" s="9">
-        <f>COUNTA(D186:AA186)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C186" t="s">
@@ -8982,7 +8989,7 @@
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B187" s="9">
-        <f>COUNTA(D187:AA187)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C187" t="s">
@@ -8994,7 +9001,7 @@
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B188" s="9">
-        <f>COUNTA(D188:AA188)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C188" t="s">
@@ -9006,7 +9013,7 @@
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B189" s="9">
-        <f>COUNTA(D189:AA189)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C189" t="s">
@@ -9018,7 +9025,7 @@
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B190" s="9">
-        <f>COUNTA(D190:AA190)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C190" t="s">
@@ -9030,7 +9037,7 @@
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B191" s="9">
-        <f>COUNTA(D191:AA191)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C191" t="s">
@@ -9042,7 +9049,7 @@
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B192" s="9">
-        <f>COUNTA(D192:AA192)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C192" t="s">
@@ -9054,7 +9061,7 @@
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B193" s="9">
-        <f>COUNTA(D193:AA193)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C193" t="s">
@@ -9066,7 +9073,7 @@
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B194" s="9">
-        <f>COUNTA(D194:AA194)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C194" t="s">
@@ -9078,7 +9085,7 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B195" s="9">
-        <f>COUNTA(D195:AA195)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C195" t="s">
@@ -9090,7 +9097,7 @@
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B196" s="9">
-        <f>COUNTA(D196:AA196)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C196" t="s">
@@ -9102,7 +9109,7 @@
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B197" s="9">
-        <f>COUNTA(D197:AA197)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C197" t="s">
@@ -9114,7 +9121,7 @@
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B198" s="9">
-        <f>COUNTA(D198:AA198)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C198" t="s">
@@ -9126,7 +9133,7 @@
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B199" s="9">
-        <f>COUNTA(D199:AA199)</f>
+        <f t="shared" ref="B199:B262" si="3">COUNTA(D199:AA199)</f>
         <v>1</v>
       </c>
       <c r="C199" t="s">
@@ -9138,7 +9145,7 @@
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B200" s="9">
-        <f>COUNTA(D200:AA200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C200" t="s">
@@ -9150,7 +9157,7 @@
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B201" s="9">
-        <f>COUNTA(D201:AA201)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C201" t="s">
@@ -9162,7 +9169,7 @@
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B202" s="9">
-        <f>COUNTA(D202:AA202)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C202" t="s">
@@ -9174,7 +9181,7 @@
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B203" s="9">
-        <f>COUNTA(D203:AA203)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C203" t="s">
@@ -9186,7 +9193,7 @@
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B204" s="9">
-        <f>COUNTA(D204:AA204)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C204" t="s">
@@ -9198,7 +9205,7 @@
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B205" s="9">
-        <f>COUNTA(D205:AA205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C205" t="s">
@@ -9210,7 +9217,7 @@
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B206" s="9">
-        <f>COUNTA(D206:AA206)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C206" s="2" t="s">
@@ -9222,7 +9229,7 @@
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B207" s="9">
-        <f>COUNTA(D207:AA207)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C207" t="s">
@@ -9234,7 +9241,7 @@
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B208" s="9">
-        <f>COUNTA(D208:AA208)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C208" t="s">
@@ -9246,7 +9253,7 @@
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B209" s="9">
-        <f>COUNTA(D209:AA209)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C209" t="s">
@@ -9258,7 +9265,7 @@
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B210" s="9">
-        <f>COUNTA(D210:AA210)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C210" t="s">
@@ -9270,7 +9277,7 @@
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B211" s="9">
-        <f>COUNTA(D211:AA211)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C211" t="s">
@@ -9282,7 +9289,7 @@
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B212" s="9">
-        <f>COUNTA(D212:AA212)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C212" s="7" t="s">
@@ -9294,7 +9301,7 @@
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B213" s="9">
-        <f>COUNTA(D213:AA213)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C213" t="s">
@@ -9306,7 +9313,7 @@
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B214" s="9">
-        <f>COUNTA(D214:AA214)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C214" t="s">
@@ -9318,7 +9325,7 @@
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B215" s="9">
-        <f>COUNTA(D215:AA215)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C215" t="s">
@@ -9330,7 +9337,7 @@
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B216" s="9">
-        <f>COUNTA(D216:AA216)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C216" t="s">
@@ -9342,7 +9349,7 @@
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B217" s="9">
-        <f>COUNTA(D217:AA217)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C217" t="s">
@@ -9354,7 +9361,7 @@
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B218" s="9">
-        <f>COUNTA(D218:AA218)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C218" t="s">
@@ -9366,7 +9373,7 @@
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B219" s="9">
-        <f>COUNTA(D219:AA219)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C219" s="2" t="s">
@@ -9378,7 +9385,7 @@
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B220" s="9">
-        <f>COUNTA(D220:AA220)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C220" s="2" t="s">
@@ -9390,7 +9397,7 @@
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B221" s="9">
-        <f>COUNTA(D221:AA221)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C221" t="s">
@@ -9402,7 +9409,7 @@
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B222" s="9">
-        <f>COUNTA(D222:AA222)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C222" t="s">
@@ -9414,7 +9421,7 @@
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B223" s="9">
-        <f>COUNTA(D223:AA223)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C223" t="s">
@@ -9426,7 +9433,7 @@
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B224" s="9">
-        <f>COUNTA(D224:AA224)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C224" t="s">
@@ -9438,7 +9445,7 @@
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B225" s="9">
-        <f>COUNTA(D225:AA225)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C225" t="s">
@@ -9450,7 +9457,7 @@
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B226" s="9">
-        <f>COUNTA(D226:AA226)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C226" t="s">
@@ -9462,7 +9469,7 @@
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B227" s="9">
-        <f>COUNTA(D227:AA227)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C227" t="s">
@@ -9474,7 +9481,7 @@
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B228" s="9">
-        <f>COUNTA(D228:AA228)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C228" t="s">
@@ -9486,7 +9493,7 @@
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B229" s="9">
-        <f>COUNTA(D229:AA229)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C229" t="s">
@@ -9498,7 +9505,7 @@
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B230" s="9">
-        <f>COUNTA(D230:AA230)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C230" t="s">
@@ -9510,7 +9517,7 @@
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B231" s="9">
-        <f>COUNTA(D231:AA231)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C231" t="s">
@@ -9522,7 +9529,7 @@
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B232" s="9">
-        <f>COUNTA(D232:AA232)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C232" t="s">
@@ -9534,7 +9541,7 @@
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B233" s="9">
-        <f>COUNTA(D233:AA233)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C233" t="s">
@@ -9546,7 +9553,7 @@
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B234" s="9">
-        <f>COUNTA(D234:AA234)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C234" t="s">
@@ -9558,7 +9565,7 @@
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B235" s="9">
-        <f>COUNTA(D235:AA235)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C235" t="s">
@@ -9570,7 +9577,7 @@
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B236" s="9">
-        <f>COUNTA(D236:AA236)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C236" s="2" t="s">
@@ -9582,7 +9589,7 @@
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B237" s="9">
-        <f>COUNTA(D237:AA237)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C237" t="s">
@@ -9594,7 +9601,7 @@
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B238" s="9">
-        <f>COUNTA(D238:AA238)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C238" t="s">
@@ -9606,7 +9613,7 @@
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B239" s="9">
-        <f>COUNTA(D239:AA239)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C239" t="s">
@@ -9618,7 +9625,7 @@
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B240" s="9">
-        <f>COUNTA(D240:AA240)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C240" t="s">
@@ -9630,7 +9637,7 @@
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B241" s="9">
-        <f>COUNTA(D241:AA241)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C241" s="2" t="s">
@@ -9642,7 +9649,7 @@
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B242" s="9">
-        <f>COUNTA(D242:AA242)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C242" t="s">
@@ -9654,7 +9661,7 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B243" s="9">
-        <f>COUNTA(D243:AA243)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C243" t="s">
@@ -9666,7 +9673,7 @@
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B244" s="9">
-        <f>COUNTA(D244:AA244)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C244" t="s">
@@ -9678,7 +9685,7 @@
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B245" s="9">
-        <f>COUNTA(D245:AA245)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C245" t="s">
@@ -9690,7 +9697,7 @@
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B246" s="9">
-        <f>COUNTA(D246:AA246)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C246" t="s">
@@ -9702,7 +9709,7 @@
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B247" s="9">
-        <f>COUNTA(D247:AA247)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C247" t="s">
@@ -9714,7 +9721,7 @@
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B248" s="9">
-        <f>COUNTA(D248:AA248)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C248" t="s">
@@ -9726,7 +9733,7 @@
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B249" s="9">
-        <f>COUNTA(D249:AA249)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C249" t="s">
@@ -9738,7 +9745,7 @@
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B250" s="9">
-        <f>COUNTA(D250:AA250)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C250" t="s">
@@ -9750,7 +9757,7 @@
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B251" s="9">
-        <f>COUNTA(D251:AA251)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C251" t="s">
@@ -9762,7 +9769,7 @@
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B252" s="9">
-        <f>COUNTA(D252:AA252)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C252" s="2" t="s">
@@ -9774,7 +9781,7 @@
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B253" s="9">
-        <f>COUNTA(D253:AA253)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C253" t="s">
@@ -9786,7 +9793,7 @@
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B254" s="9">
-        <f>COUNTA(D254:AA254)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C254" t="s">
@@ -9798,7 +9805,7 @@
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B255" s="9">
-        <f>COUNTA(D255:AA255)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C255" t="s">
@@ -9810,7 +9817,7 @@
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B256" s="9">
-        <f>COUNTA(D256:AA256)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C256" t="s">
@@ -9822,7 +9829,7 @@
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B257" s="9">
-        <f>COUNTA(D257:AA257)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C257" t="s">
@@ -9834,7 +9841,7 @@
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B258" s="9">
-        <f>COUNTA(D258:AA258)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C258" t="s">
@@ -9846,7 +9853,7 @@
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B259" s="9">
-        <f>COUNTA(D259:AA259)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C259" t="s">
@@ -9858,7 +9865,7 @@
     </row>
     <row r="260" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B260" s="9">
-        <f>COUNTA(D260:AA260)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C260" t="s">
@@ -9870,7 +9877,7 @@
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B261" s="9">
-        <f>COUNTA(D261:AA261)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C261" t="s">
@@ -9882,7 +9889,7 @@
     </row>
     <row r="262" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B262" s="9">
-        <f>COUNTA(D262:AA262)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C262" t="s">
@@ -9894,7 +9901,7 @@
     </row>
     <row r="263" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B263" s="9">
-        <f>COUNTA(D263:AA263)</f>
+        <f t="shared" ref="B263:B296" si="4">COUNTA(D263:AA263)</f>
         <v>1</v>
       </c>
       <c r="C263" t="s">
@@ -9906,7 +9913,7 @@
     </row>
     <row r="264" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B264" s="9">
-        <f>COUNTA(D264:AA264)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C264" t="s">
@@ -9918,7 +9925,7 @@
     </row>
     <row r="265" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B265" s="9">
-        <f>COUNTA(D265:AA265)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C265" t="s">
@@ -9930,7 +9937,7 @@
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B266" s="9">
-        <f>COUNTA(D266:AA266)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C266" t="s">
@@ -9942,7 +9949,7 @@
     </row>
     <row r="267" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B267" s="9">
-        <f>COUNTA(D267:AA267)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C267" t="s">
@@ -9954,7 +9961,7 @@
     </row>
     <row r="268" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B268" s="9">
-        <f>COUNTA(D268:AA268)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C268" t="s">
@@ -9966,7 +9973,7 @@
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B269" s="9">
-        <f>COUNTA(D269:AA269)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C269" t="s">
@@ -9978,7 +9985,7 @@
     </row>
     <row r="270" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B270" s="9">
-        <f>COUNTA(D270:AA270)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C270" t="s">
@@ -9990,7 +9997,7 @@
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B271" s="9">
-        <f>COUNTA(D271:AA271)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C271" t="s">
@@ -10002,7 +10009,7 @@
     </row>
     <row r="272" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B272" s="9">
-        <f>COUNTA(D272:AA272)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C272" t="s">
@@ -10014,7 +10021,7 @@
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B273" s="9">
-        <f>COUNTA(D273:AA273)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C273" t="s">
@@ -10026,7 +10033,7 @@
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B274" s="9">
-        <f>COUNTA(D274:AA274)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C274" t="s">
@@ -10038,7 +10045,7 @@
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B275" s="9">
-        <f>COUNTA(D275:AA275)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C275" t="s">
@@ -10050,7 +10057,7 @@
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B276" s="9">
-        <f>COUNTA(D276:AA276)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C276" t="s">
@@ -10062,7 +10069,7 @@
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B277" s="9">
-        <f>COUNTA(D277:AA277)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C277" s="11" t="s">
@@ -10074,7 +10081,7 @@
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B278" s="9">
-        <f>COUNTA(D278:AA278)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C278" t="s">
@@ -10086,7 +10093,7 @@
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B279" s="9">
-        <f>COUNTA(D279:AA279)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C279" t="s">
@@ -10098,7 +10105,7 @@
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B280" s="9">
-        <f>COUNTA(D280:AA280)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C280" t="s">
@@ -10110,7 +10117,7 @@
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B281" s="9">
-        <f>COUNTA(D281:AA281)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C281" t="s">
@@ -10122,7 +10129,7 @@
     </row>
     <row r="282" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B282" s="9">
-        <f>COUNTA(D282:AA282)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C282" t="s">
@@ -10134,7 +10141,7 @@
     </row>
     <row r="283" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B283" s="9">
-        <f>COUNTA(D283:AA283)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C283" t="s">
@@ -10146,7 +10153,7 @@
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B284" s="9">
-        <f>COUNTA(D284:AA284)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C284" t="s">
@@ -10158,7 +10165,7 @@
     </row>
     <row r="285" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B285" s="9">
-        <f>COUNTA(D285:AA285)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C285" t="s">
@@ -10170,7 +10177,7 @@
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B286" s="9">
-        <f>COUNTA(D286:AA286)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C286" t="s">
@@ -10182,7 +10189,7 @@
     </row>
     <row r="287" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B287" s="9">
-        <f>COUNTA(D287:AA287)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C287" t="s">
@@ -10194,7 +10201,7 @@
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B288" s="9">
-        <f>COUNTA(D288:AA288)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C288" t="s">
@@ -10206,7 +10213,7 @@
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B289" s="9">
-        <f>COUNTA(D289:AA289)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C289" t="s">
@@ -10218,7 +10225,7 @@
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B290" s="9">
-        <f>COUNTA(D290:AA290)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C290" t="s">
@@ -10230,7 +10237,7 @@
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B291" s="9">
-        <f>COUNTA(D291:AA291)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C291" t="s">
@@ -10242,7 +10249,7 @@
     </row>
     <row r="292" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B292" s="9">
-        <f>COUNTA(D292:AA292)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C292" t="s">
@@ -10254,7 +10261,7 @@
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B293" s="9">
-        <f>COUNTA(D293:AA293)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C293" t="s">
@@ -10266,7 +10273,7 @@
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B294" s="9">
-        <f>COUNTA(D294:AA294)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C294" t="s">
@@ -10278,7 +10285,7 @@
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B295" s="9">
-        <f>COUNTA(D295:AA295)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C295" t="s">
@@ -10290,7 +10297,7 @@
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B296" s="9">
-        <f>COUNTA(D296:AA296)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C296" t="s">
@@ -10313,8 +10320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A0738F-DFD0-4775-9DE7-D468DC9E8D37}">
   <dimension ref="C3:H61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11064,10 +11071,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB39E36-9C50-466B-9635-5C6100481B4D}">
-  <dimension ref="B3:D294"/>
+  <dimension ref="B3:D293"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B83"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11324,158 +11331,156 @@
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>228</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>32</v>
+      <c r="B60" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B61" s="6" t="s">
-        <v>1</v>
+      <c r="B61" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>352</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>57</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>205</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>348</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>212</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>115</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
         <v>247</v>
       </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="13"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="13"/>
@@ -12045,10 +12050,10 @@
       <c r="B273" s="13"/>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B274" s="13"/>
+      <c r="B274" s="14"/>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B275" s="14"/>
+      <c r="B275" s="13"/>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="13"/>
@@ -12103,9 +12108,6 @@
     </row>
     <row r="293" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B293" s="13"/>
-    </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B294" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12114,10 +12116,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67919AD-33E1-48BC-91D6-EA42D90D84E5}">
-  <dimension ref="B3:D293"/>
+  <dimension ref="B3:D292"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12319,457 +12321,457 @@
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>228</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>328</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>146</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>360</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>222</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>362</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>47</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>160</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>44</v>
+        <v>373</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>373</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>34</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>350</v>
+        <v>374</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>374</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>202</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>36</v>
+        <v>389</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>389</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>32</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>375</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>96</v>
+        <v>376</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>376</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>152</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>184</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>390</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>125</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>391</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>313</v>
+        <v>377</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>377</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>28</v>
+        <v>378</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
-        <v>378</v>
+      <c r="B99" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B100" s="2" t="s">
-        <v>64</v>
+      <c r="B100" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
-        <v>135</v>
+      <c r="B104" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="6" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B106" s="6" t="s">
-        <v>1</v>
+      <c r="B106" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
-        <v>27</v>
+        <v>339</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
-        <v>339</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
-        <v>379</v>
+        <v>352</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>352</v>
+        <v>392</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
-        <v>394</v>
+        <v>185</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
-        <v>185</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>5</v>
+        <v>395</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
-        <v>395</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
-        <v>145</v>
+        <v>315</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
-        <v>315</v>
+        <v>380</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
-        <v>380</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
-        <v>192</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.3">
@@ -12779,808 +12781,831 @@
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
-        <v>140</v>
+        <v>186</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B140" t="s">
-        <v>189</v>
+      <c r="B140" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B141" s="3" t="s">
-        <v>164</v>
+      <c r="B141" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
-        <v>333</v>
+        <v>86</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
-        <v>76</v>
+        <v>229</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
-        <v>230</v>
+        <v>73</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
-        <v>224</v>
+        <v>396</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
-        <v>397</v>
+        <v>57</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B168" t="s">
-        <v>82</v>
+      <c r="B168" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B169" s="2" t="s">
-        <v>65</v>
+      <c r="B169" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
-        <v>121</v>
+        <v>398</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
-        <v>398</v>
+        <v>22</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B174" t="s">
-        <v>178</v>
+      <c r="B174" s="7" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B175" s="7" t="s">
-        <v>335</v>
+      <c r="B175" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
-        <v>13</v>
+        <v>232</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
-        <v>232</v>
+        <v>111</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
-        <v>111</v>
+        <v>367</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
-        <v>367</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B186" t="s">
-        <v>161</v>
+      <c r="B186" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="2" t="s">
-        <v>63</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B188" s="2" t="s">
-        <v>248</v>
+      <c r="B188" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
-        <v>53</v>
+        <v>381</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
-        <v>381</v>
+        <v>78</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
-        <v>41</v>
+        <v>205</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
-        <v>205</v>
+        <v>348</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
-        <v>348</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
-        <v>218</v>
+        <v>91</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
-        <v>30</v>
+        <v>207</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" t="s">
-        <v>207</v>
+        <v>95</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
-        <v>89</v>
+        <v>208</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" t="s">
-        <v>175</v>
+        <v>50</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>50</v>
+        <v>345</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" t="s">
-        <v>345</v>
+        <v>94</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B212" t="s">
+      <c r="B212" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B213" s="2" t="s">
-        <v>127</v>
+      <c r="B213" s="6" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B214" s="6" t="s">
-        <v>168</v>
+      <c r="B214" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" t="s">
-        <v>10</v>
+        <v>233</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" t="s">
-        <v>210</v>
+        <v>400</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B220" t="s">
-        <v>400</v>
+      <c r="B220" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B221" s="2" t="s">
-        <v>169</v>
+      <c r="B221" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" t="s">
-        <v>7</v>
+        <v>401</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" t="s">
-        <v>167</v>
+        <v>234</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" t="s">
-        <v>235</v>
+        <v>402</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
-        <v>402</v>
+        <v>21</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" t="s">
-        <v>87</v>
+        <v>403</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" t="s">
-        <v>403</v>
+        <v>51</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B233" t="s">
-        <v>51</v>
+      <c r="B233" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B234" s="2" t="s">
-        <v>66</v>
+      <c r="B234" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" t="s">
-        <v>122</v>
+        <v>404</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" t="s">
-        <v>404</v>
+        <v>337</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" t="s">
-        <v>341</v>
+        <v>55</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" t="s">
-        <v>108</v>
+        <v>316</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" t="s">
-        <v>316</v>
+        <v>99</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" t="s">
-        <v>212</v>
+        <v>332</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" t="s">
-        <v>332</v>
+        <v>115</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" t="s">
-        <v>123</v>
+        <v>214</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" t="s">
-        <v>214</v>
+        <v>107</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" t="s">
-        <v>46</v>
+        <v>174</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B254" t="s">
-        <v>174</v>
+      <c r="B254" s="11" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B255" s="11" t="s">
-        <v>318</v>
+      <c r="B255" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" t="s">
-        <v>324</v>
+        <v>35</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B261" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B262" t="s">
-        <v>196</v>
+        <v>90</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B263" t="s">
-        <v>90</v>
+        <v>354</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B264" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B265" t="s">
-        <v>215</v>
+        <v>49</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B266" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B267" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B268" t="s">
-        <v>103</v>
+        <v>190</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B269" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B270" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B271" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B272" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" t="s">
-        <v>236</v>
+        <v>325</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" t="s">
-        <v>325</v>
+        <v>33</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" t="s">
-        <v>33</v>
+        <v>244</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B281" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="282" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B282" t="s">
-        <v>247</v>
+      <c r="B282" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B283" s="3" t="s">
-        <v>58</v>
+      <c r="B283" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B284" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="285" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B285" t="s">
-        <v>217</v>
+        <v>136</v>
       </c>
     </row>
     <row r="286" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B286" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
     </row>
     <row r="287" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>162</v>
+        <v>334</v>
       </c>
     </row>
     <row r="288" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B288" t="s">
-        <v>334</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B289" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="290" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B290" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="291" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B291" t="s">
-        <v>80</v>
+        <v>317</v>
       </c>
     </row>
     <row r="292" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B292" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B293" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B294">
-    <sortCondition ref="B2:B294"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B293">
+    <sortCondition ref="B2:B293"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB98909-40BF-4210-A56F-670C09F178CD}">
+  <dimension ref="B4:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5">
+        <v>19962</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GEO data - Update. Need to refine PreProcessing and Loading based on model we choose.
</commit_message>
<xml_diff>
--- a/Supplement/genesReferencesFeatureSetsNumbered.xlsx
+++ b/Supplement/genesReferencesFeatureSetsNumbered.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\000_Projecten\HogeschoolRotterdam\ExploratoryDevelopmentCapstone\UITZOEKEN_Supplement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\000_Projecten\HogeschoolRotterdam\ExploratoryDevelopmentCapstone\Supplement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220BEED5-F5B3-45A5-B8BE-2E9FE11A6363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB91505-C7AF-43D6-9505-A7B1520E3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="419">
   <si>
     <t>s10911-023-09540-2</t>
   </si>
@@ -1285,6 +1285,21 @@
   </si>
   <si>
     <t>B7-H1</t>
+  </si>
+  <si>
+    <t>IGJ</t>
+  </si>
+  <si>
+    <t>SCYC2</t>
+  </si>
+  <si>
+    <t>DARC</t>
+  </si>
+  <si>
+    <t>WDR67</t>
+  </si>
+  <si>
+    <t>FIGF</t>
   </si>
 </sst>
 </file>
@@ -10297,10 +10312,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A0738F-DFD0-4775-9DE7-D468DC9E8D37}">
-  <dimension ref="C3:H62"/>
+  <dimension ref="C3:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10344,173 +10359,173 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>290</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>251</v>
+        <v>287</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>352</v>
+        <v>251</v>
       </c>
       <c r="D11" t="s">
-        <v>353</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D12" t="s">
-        <v>355</v>
-      </c>
-      <c r="E12" t="s">
-        <v>356</v>
-      </c>
-      <c r="F12" t="s">
-        <v>357</v>
-      </c>
-      <c r="G12" t="s">
-        <v>358</v>
-      </c>
-      <c r="H12" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="D13" t="s">
-        <v>366</v>
+        <v>355</v>
+      </c>
+      <c r="E13" t="s">
+        <v>356</v>
+      </c>
+      <c r="F13" t="s">
+        <v>357</v>
+      </c>
+      <c r="G13" t="s">
+        <v>358</v>
+      </c>
+      <c r="H13" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>301</v>
+        <v>365</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
-      </c>
-      <c r="E14" t="s">
-        <v>241</v>
-      </c>
-      <c r="F14" t="s">
-        <v>242</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>253</v>
+        <v>301</v>
       </c>
       <c r="D15" t="s">
-        <v>304</v>
+        <v>240</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>241</v>
       </c>
       <c r="F15" t="s">
-        <v>305</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>304</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D21" t="s">
-        <v>279</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
@@ -10518,96 +10533,96 @@
         <v>262</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>381</v>
+        <v>309</v>
       </c>
       <c r="D28" t="s">
-        <v>382</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>294</v>
+        <v>381</v>
       </c>
       <c r="D29" t="s">
-        <v>295</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="D31" t="s">
-        <v>265</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="D32" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
-      </c>
-      <c r="E33" t="s">
-        <v>186</v>
-      </c>
-      <c r="F33" t="s">
-        <v>187</v>
-      </c>
-      <c r="G33" t="s">
-        <v>188</v>
-      </c>
-      <c r="H33" t="s">
-        <v>189</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
+        <v>185</v>
+      </c>
+      <c r="E34" t="s">
+        <v>186</v>
+      </c>
+      <c r="F34" t="s">
+        <v>187</v>
+      </c>
+      <c r="G34" t="s">
+        <v>188</v>
+      </c>
+      <c r="H34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D35" t="s">
         <v>228</v>
@@ -10615,242 +10630,282 @@
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>257</v>
+        <v>303</v>
       </c>
       <c r="D37" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D38" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>298</v>
+        <v>259</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>268</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D43" t="s">
-        <v>267</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>398</v>
+        <v>266</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>297</v>
+        <v>398</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>269</v>
+        <v>329</v>
       </c>
       <c r="D48" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>249</v>
+        <v>297</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>248</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="E51" s="5"/>
+        <v>249</v>
+      </c>
+      <c r="D51" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>343</v>
+        <v>248</v>
       </c>
       <c r="D52" t="s">
-        <v>344</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>284</v>
-      </c>
-      <c r="D53" t="s">
-        <v>127</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>272</v>
+        <v>343</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="D55" t="s">
-        <v>254</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>335</v>
+        <v>272</v>
       </c>
       <c r="D56" t="s">
-        <v>336</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>318</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>317</v>
+        <v>252</v>
+      </c>
+      <c r="D57" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="D58" t="s">
-        <v>193</v>
-      </c>
-      <c r="E58" t="s">
-        <v>194</v>
-      </c>
-      <c r="F58" t="s">
-        <v>195</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>273</v>
-      </c>
-      <c r="D59" t="s">
-        <v>46</v>
+        <v>318</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="D60" t="s">
-        <v>243</v>
-      </c>
-      <c r="E60" t="s">
-        <v>244</v>
-      </c>
-      <c r="F60" t="s">
-        <v>245</v>
-      </c>
-      <c r="G60" t="s">
-        <v>246</v>
-      </c>
-      <c r="H60" t="s">
-        <v>127</v>
+        <v>417</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D61" t="s">
-        <v>292</v>
+        <v>193</v>
+      </c>
+      <c r="E61" t="s">
+        <v>194</v>
+      </c>
+      <c r="F61" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
+        <v>273</v>
+      </c>
+      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>302</v>
+      </c>
+      <c r="D63" t="s">
+        <v>243</v>
+      </c>
+      <c r="E63" t="s">
+        <v>244</v>
+      </c>
+      <c r="F63" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63" t="s">
+        <v>246</v>
+      </c>
+      <c r="H63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>246</v>
+      </c>
+      <c r="D64" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>291</v>
+      </c>
+      <c r="D65" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
         <v>275</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D66" t="s">
         <v>276</v>
       </c>
     </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" t="s">
+        <v>415</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H62">
-    <sortCondition ref="C5:C62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H66">
+    <sortCondition ref="C5:C66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>